<commit_message>
added Practice_03-Init_Container and Practice_04-Liviness-probe
</commit_message>
<xml_diff>
--- a/Kubernetes parancsok.xlsx
+++ b/Kubernetes parancsok.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programing\Git\Kubernetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
   <si>
     <t xml:space="preserve">Parancs </t>
   </si>
@@ -233,13 +233,86 @@
   </si>
   <si>
     <t>stdin: true   '133'</t>
+  </si>
+  <si>
+    <t>kubectl logs kubia-ssl -c kubia</t>
+  </si>
+  <si>
+    <t>DISPLAYING LOGS OF PODS WITH MULTIPLE CONTAINERS</t>
+  </si>
+  <si>
+    <t>kubectl logs kubia-ssl --all-containers</t>
+  </si>
+  <si>
+    <t>kubectl get pods -w</t>
+  </si>
+  <si>
+    <t>Listing pods in real time</t>
+  </si>
+  <si>
+    <t>kubectl get events -w</t>
+  </si>
+  <si>
+    <t>Events recorded after deploying a Pod object in real time</t>
+  </si>
+  <si>
+    <t>ENTERING A RUNNING INIT CONTAINER</t>
+  </si>
+  <si>
+    <t>kubectl exec -it kubia-ssl-c init-demo -- sh</t>
+  </si>
+  <si>
+    <t>DELETING A SINGLE POD</t>
+  </si>
+  <si>
+    <t>kubectl delete po kubia</t>
+  </si>
+  <si>
+    <t>DELETING MULTIPLE PODS WITH A SINGLE COMMAND</t>
+  </si>
+  <si>
+    <t>kubectl delete po kubia-init kubia-init-slow</t>
+  </si>
+  <si>
+    <t>$ kubectl delete -f kubia-ssl.yaml 
+pod "kubia-ssl" deleted</t>
+  </si>
+  <si>
+    <t>Deleting objects defined in manifest files</t>
+  </si>
+  <si>
+    <t>DELETING OBJECTS FROM MULTIPLE MANIFEST FILES</t>
+  </si>
+  <si>
+    <t>kubectl delete -f kubia.yaml,kubia-ssl.yaml</t>
+  </si>
+  <si>
+    <t>kubectl delete -f Chapter05/</t>
+  </si>
+  <si>
+    <t>You can then delete the pods using the same method</t>
+  </si>
+  <si>
+    <t>Deleting all pods</t>
+  </si>
+  <si>
+    <t>kubectl delete po --all</t>
+  </si>
+  <si>
+    <t>kubectl delete all --all</t>
+  </si>
+  <si>
+    <t>Deleting objects of most kinds</t>
+  </si>
+  <si>
+    <t>Liveness probes can only be used in the pod’s regular containers. They can’t be defined in init containers.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,8 +362,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +387,11 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -317,13 +402,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,8 +435,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -632,18 +722,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.7109375" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" customWidth="1"/>
     <col min="4" max="4" width="67.42578125" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
     <col min="11" max="11" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -664,7 +755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -677,11 +768,14 @@
       <c r="D2" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="E2" s="11" t="s">
+        <v>91</v>
+      </c>
       <c r="K2" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -711,10 +805,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>67</v>
@@ -725,202 +819,298 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>46</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>